<commit_message>
deep learning part 3 done
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smitesh\Documents\Football Data Analysis\Masters-Assignment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC11E61-F6CF-45EA-919F-27FCB96DAE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B6EBE7-0C4B-4148-90E6-0DCA1190614D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3510" windowWidth="38640" windowHeight="21120" xr2:uid="{05EEA40C-0A3B-49F9-BDA8-2F3C44A6B853}"/>
+    <workbookView xWindow="28680" yWindow="-1815" windowWidth="38640" windowHeight="21120" xr2:uid="{05EEA40C-0A3B-49F9-BDA8-2F3C44A6B853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>Module</t>
   </si>
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B2DC14-AEBF-4D39-9D44-8E91CF3B9CFE}">
-  <dimension ref="A1:AO17"/>
+  <dimension ref="A1:AO18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,16 +639,16 @@
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="1">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="2">
         <v>44992</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -746,16 +746,30 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="7">
         <v>4</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="8">
         <v>44992</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2</v>
+      </c>
+      <c r="C18" s="6">
+        <v>45009</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data viz ass2 done
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smitesh\Documents\Football Data Analysis\Masters-Assignment-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEA12A9-A5EC-462A-8788-608BD5F4498A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE045D2-36AA-46C8-9ED2-312142F212EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05EEA40C-0A3B-49F9-BDA8-2F3C44A6B853}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
   <si>
     <t>Module</t>
   </si>
@@ -108,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +133,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -146,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -156,7 +162,8 @@
     <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B2DC14-AEBF-4D39-9D44-8E91CF3B9CFE}">
-  <dimension ref="A1:AO19"/>
+  <dimension ref="A1:AO20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -719,44 +726,44 @@
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="2">
         <v>44993</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="8">
         <v>45005</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="1">
         <v>4</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="2">
         <v>44992</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -781,10 +788,24 @@
       <c r="B19" s="5">
         <v>2</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="6">
         <v>45019</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="9">
+        <v>5</v>
+      </c>
+      <c r="C20" s="10">
+        <v>44999</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>